<commit_message>
Fixed triggers and ranking
</commit_message>
<xml_diff>
--- a/data/portfolio.xlsx
+++ b/data/portfolio.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -746,7 +746,7 @@
           <t>TITAN</t>
         </is>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="2" t="n">
         <v>44965</v>
       </c>
       <c r="C15" t="n">
@@ -758,6 +758,216 @@
       <c r="E15" t="inlineStr">
         <is>
           <t>Titan company limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FCL</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C16" t="n">
+        <v>160</v>
+      </c>
+      <c r="D16" t="n">
+        <v>256.9</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Fineotex chemical limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>LTTS</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C17" t="n">
+        <v>11</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3622.04</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L&amp;t technology services limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ABBOTINDIA</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44970</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>20592.1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Abbott india limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ABBOTINDIA</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44970</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>20592.05</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Abbott india limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ABBOTINDIA</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44970</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>20591</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Abbott india limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FCL</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>255.7</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Fineotex chemical limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LTTS</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-11</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3593.85</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L&amp;t technology services limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FCL</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-165</v>
+      </c>
+      <c r="D23" t="n">
+        <v>254</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Fineotex chemical limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FCL</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C24" t="n">
+        <v>160</v>
+      </c>
+      <c r="D24" t="n">
+        <v>252.8</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Fineotex chemical limited</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>LTTS</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>44972</v>
+      </c>
+      <c r="C25" t="n">
+        <v>11</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3601.14</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L&amp;t technology services limited</t>
         </is>
       </c>
     </row>

</xml_diff>